<commit_message>
excluding useless verification when frequency equals zero and fixing the cost values
</commit_message>
<xml_diff>
--- a/MCDA - AHP (Modelo 1).xlsx
+++ b/MCDA - AHP (Modelo 1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\source\repos\thj3a\Optimizing-bus-lines-frequecy.py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19E2EC9-5F13-4EC7-BE65-4486C6B3F5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132E57B3-3371-49BD-8EB5-7CDF4F59CD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="718" firstSheet="6" activeTab="8" xr2:uid="{3B4055F7-C661-4161-8396-3DA6C25D3E4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="718" firstSheet="6" activeTab="12" xr2:uid="{3B4055F7-C661-4161-8396-3DA6C25D3E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="AHP (1) - Dados" sheetId="27" r:id="rId1"/>
@@ -3081,10 +3081,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8675F6D8-B40E-4AF8-84C0-2781B3DFF4A3}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,7 +3096,7 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>1</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>7</v>
       </c>
@@ -3121,20 +3121,17 @@
         <v>1</v>
       </c>
       <c r="C2" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D82:I82)</f>
-        <v>0.83333333333333326</v>
+        <v>3.1599501467729985</v>
       </c>
       <c r="D2" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D86:I86)</f>
-        <v>6.0578174248885484</v>
+        <v>3.0779975079782327</v>
       </c>
       <c r="E2" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D90:I90)</f>
-        <v>5.6058238631735371</v>
+        <v>3.0011146924523233</v>
       </c>
       <c r="F2" s="63"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>7</v>
       </c>
@@ -3142,19 +3139,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D83:I83)</f>
-        <v>0</v>
+        <v>2.8866902198703386</v>
       </c>
       <c r="D3" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D87:I87)</f>
-        <v>8.2838465906910717</v>
+        <v>2.722784942280807</v>
       </c>
       <c r="E3" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D91:I91)</f>
-        <v>7.7725229147852213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.5690193112289874</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>7</v>
       </c>
@@ -3162,19 +3156,17 @@
         <v>4</v>
       </c>
       <c r="C4" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D84:I84)</f>
-        <v>3.3298847872958746</v>
+        <v>2.4957259216205738</v>
       </c>
       <c r="D4" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D88:I88)</f>
-        <v>3.2446641746448996</v>
+        <v>2.0568042553303996</v>
       </c>
       <c r="E4" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D92:I92)</f>
-        <v>3.1726833199033035</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.8603841043378722</v>
+      </c>
+      <c r="G4" s="63"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>7</v>
       </c>
@@ -3182,19 +3174,16 @@
         <v>6</v>
       </c>
       <c r="C5" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D85:I85)</f>
-        <v>4.1873438146415811</v>
+        <v>2.4603171789263647</v>
       </c>
       <c r="D5" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D89:I89)</f>
-        <v>4.0169025893396304</v>
+        <v>1.9686013461577696</v>
       </c>
       <c r="E5" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D93:I93)</f>
-        <v>3.8729408798564386</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.5073044530023123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>8</v>
       </c>
@@ -3202,19 +3191,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D94:I94)</f>
-        <v>5.4290115553182652</v>
+        <v>3.2048700270538779</v>
       </c>
       <c r="D6" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D98:I98)</f>
-        <v>6.1263858349009546</v>
+        <v>3.108456814988708</v>
       </c>
       <c r="E6" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D102:I102)</f>
-        <v>5.6165499801043275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.0113573283194555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -3222,19 +3208,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D95:I95)</f>
-        <v>7.3406377863356456</v>
+        <v>2.7543077582098752</v>
       </c>
       <c r="D7" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D99:I99)</f>
-        <v>8.5533658723763484</v>
+        <v>2.5614813340795353</v>
       </c>
       <c r="E7" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D103:I103)</f>
-        <v>7.9552787568480738</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.3672823607410303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -3242,19 +3225,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D96:I96)</f>
-        <v>3.374804667576754</v>
+        <v>2.5642943316329809</v>
       </c>
       <c r="D8" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D100:I100)</f>
-        <v>3.2751234816553749</v>
+        <v>2.06753037226119</v>
       </c>
       <c r="E8" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D104:I104)</f>
-        <v>3.1829259557704357</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.6791324255841789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -3262,19 +3242,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D97:I97)</f>
-        <v>4.0549613529811177</v>
+        <v>2.7298364606116414</v>
       </c>
       <c r="D9" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D101:I101)</f>
-        <v>3.8555989811383591</v>
+        <v>2.1513571882206222</v>
       </c>
       <c r="E9" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D105:I105)</f>
-        <v>3.6712039293684815</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.5687602682051056</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>9</v>
       </c>
@@ -3282,19 +3259,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D106:I106)</f>
-        <v>5.2477598765645714</v>
+        <v>3.2497899073347574</v>
       </c>
       <c r="D10" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D110:I110)</f>
-        <v>6.3060653560244724</v>
+        <v>3.1389161219991832</v>
       </c>
       <c r="E10" s="48">
-        <f>SUM('AHP (1) - Normalização Dados'!D114:I114)</f>
-        <v>5.8494983192573393</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.0215999641865876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
@@ -3302,19 +3276,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D107:I107)</f>
-        <v>7.4020936015384393</v>
+        <v>3.0663697409938564</v>
       </c>
       <c r="D11" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D111:I111)</f>
-        <v>8.8228851540616251</v>
+        <v>2.844622170322709</v>
       </c>
       <c r="E11" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D115:I115)</f>
-        <v>8.1380345989109273</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.6099898546975169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
@@ -3322,19 +3293,16 @@
         <v>4</v>
       </c>
       <c r="C12" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D108:I108)</f>
-        <v>3.4197245478576335</v>
+        <v>2.7439738527564987</v>
       </c>
       <c r="D12" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D112:I112)</f>
-        <v>3.3055827886658502</v>
+        <v>2.3004787114142031</v>
       </c>
       <c r="E12" s="16">
-        <f>SUM('AHP (1) - Normalização Dados'!D116:I116)</f>
-        <v>3.1931685916375678</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.831214080163819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>9</v>
       </c>
@@ -3342,17 +3310,18 @@
         <v>6</v>
       </c>
       <c r="C13" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D109:I109)</f>
-        <v>4.3670233357650989</v>
+        <v>2.9993557422969186</v>
       </c>
       <c r="D13" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D113:I113)</f>
-        <v>4.1387398173815324</v>
+        <v>2.3341130302834747</v>
       </c>
       <c r="E13" s="17">
-        <f>SUM('AHP (1) - Normalização Dados'!D117:I117)</f>
-        <v>3.9139114233249681</v>
-      </c>
+        <v>1.6302160834078991</v>
+      </c>
+      <c r="J13" s="63"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="63"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:E5">
@@ -3392,6 +3361,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11462,8 +11432,8 @@
   </sheetPr>
   <dimension ref="B2:N38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>